<commit_message>
Deploying to gh-pages from  @ 8ac870eac37250c3e09f9221d42c8cb9819cfd6f 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/2.1.1.xlsx
+++ b/en/downloads/data-excel/2.1.1.xlsx
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -399,15 +399,20 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -693,10 +698,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -706,8 +711,8 @@
     <col min="3" max="3" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="26" t="s">
@@ -717,7 +722,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
@@ -728,19 +733,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="4">
@@ -809,8 +814,11 @@
       <c r="Y4" s="4">
         <v>2021</v>
       </c>
+      <c r="Z4" s="39">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>14</v>
       </c>
@@ -886,9 +894,12 @@
       <c r="Y5" s="15">
         <v>46.69</v>
       </c>
+      <c r="Z5" s="15">
+        <v>47.345690436648667</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -963,8 +974,11 @@
       <c r="Y6" s="20">
         <v>52.52</v>
       </c>
+      <c r="Z6" s="20">
+        <v>55.294335329978139</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>43</v>
       </c>
@@ -1040,8 +1054,11 @@
       <c r="Y7" s="20">
         <v>43.22</v>
       </c>
+      <c r="Z7" s="20">
+        <v>42.721146742902135</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>15</v>
       </c>
@@ -1117,8 +1134,11 @@
       <c r="Y8" s="20">
         <v>51.31</v>
       </c>
+      <c r="Z8" s="20">
+        <v>56.732662465911261</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>16</v>
       </c>
@@ -1194,8 +1214,11 @@
       <c r="Y9" s="20">
         <v>41.31</v>
       </c>
+      <c r="Z9" s="20">
+        <v>39.351829932862628</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>17</v>
       </c>
@@ -1271,8 +1294,11 @@
       <c r="Y10" s="20">
         <v>52.43</v>
       </c>
+      <c r="Z10" s="20">
+        <v>43.952035422218046</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>18</v>
       </c>
@@ -1348,8 +1374,11 @@
       <c r="Y11" s="20">
         <v>49.27</v>
       </c>
+      <c r="Z11" s="20">
+        <v>57.461907794486649</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>19</v>
       </c>
@@ -1425,8 +1454,11 @@
       <c r="Y12" s="20">
         <v>31.68</v>
       </c>
+      <c r="Z12" s="20">
+        <v>32.073481974524846</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
         <v>20</v>
       </c>
@@ -1502,8 +1534,11 @@
       <c r="Y13" s="20">
         <v>35.590000000000003</v>
       </c>
+      <c r="Z13" s="20">
+        <v>33.564455947162017</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
         <v>21</v>
       </c>
@@ -1579,8 +1614,11 @@
       <c r="Y14" s="20">
         <v>55.28</v>
       </c>
+      <c r="Z14" s="20">
+        <v>55.803694659011171</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>22</v>
       </c>
@@ -1656,8 +1694,11 @@
       <c r="Y15" s="20">
         <v>61.02</v>
       </c>
+      <c r="Z15" s="20">
+        <v>63.920911723512503</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>23</v>
       </c>
@@ -1707,6 +1748,9 @@
       <c r="Y16" s="25">
         <v>48.72</v>
       </c>
+      <c r="Z16" s="25">
+        <v>52.521342498654128</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>